<commit_message>
updated plots. Started to write a post
</commit_message>
<xml_diff>
--- a/_posts/catholic/plotBible/NewTestamentReference.xlsx
+++ b/_posts/catholic/plotBible/NewTestamentReference.xlsx
@@ -8,29 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savey/repos/stefanavey.github.io/_posts/catholic/plotBible/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF25AEBB-6472-174A-ADE9-34BD034848F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1A32D5-32DD-D647-BC32-BBE0164BBD08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{4455D4D6-E91F-4A4F-B0DD-5AB0CFB08E3C}"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4455D4D6-E91F-4A4F-B0DD-5AB0CFB08E3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gospels" sheetId="1" r:id="rId1"/>
+    <sheet name="NT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="36">
   <si>
     <t>Matt</t>
   </si>
@@ -83,12 +79,6 @@
     <t>Col</t>
   </si>
   <si>
-    <t>1Thess</t>
-  </si>
-  <si>
-    <t>2Thess</t>
-  </si>
-  <si>
     <t>1 Tim</t>
   </si>
   <si>
@@ -104,15 +94,6 @@
     <t>Heb</t>
   </si>
   <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>1 Peter</t>
-  </si>
-  <si>
-    <t>2 Peter</t>
-  </si>
-  <si>
     <t>1 John</t>
   </si>
   <si>
@@ -126,9 +107,6 @@
   </si>
   <si>
     <t>Rev</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <r>
@@ -185,6 +163,21 @@
   </si>
   <si>
     <t>Total # Words</t>
+  </si>
+  <si>
+    <t>1 Thess</t>
+  </si>
+  <si>
+    <t>2 Thess</t>
+  </si>
+  <si>
+    <t>Jas</t>
+  </si>
+  <si>
+    <t>1 Pet</t>
+  </si>
+  <si>
+    <t>2 Pet</t>
   </si>
 </sst>
 </file>
@@ -241,12 +234,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,9 +553,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306B2B8D-C994-134D-B0CA-E3566FBBD918}">
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -571,10 +563,10 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1">
         <v>1</v>
@@ -661,10 +653,10 @@
         <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -1059,158 +1051,663 @@
         <v>15635</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D654D1DD-4080-0D45-B345-509C6D6F1D13}">
+  <dimension ref="A1:AF24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3">
+        <v>42</v>
+      </c>
+      <c r="H2" s="3">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3">
+        <v>60</v>
+      </c>
+      <c r="J2" s="3">
+        <v>40</v>
+      </c>
+      <c r="K2" s="3">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3">
+        <v>48</v>
+      </c>
+      <c r="M2" s="3">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3">
+        <v>25</v>
+      </c>
+      <c r="O2" s="3">
+        <v>52</v>
+      </c>
+      <c r="P2" s="3">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>41</v>
+      </c>
+      <c r="R2" s="3">
+        <v>40</v>
+      </c>
+      <c r="S2" s="3">
+        <v>34</v>
+      </c>
+      <c r="T2" s="3">
+        <v>28</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="3">
+        <v>38</v>
+      </c>
+      <c r="W2" s="3">
+        <v>40</v>
+      </c>
+      <c r="X2" s="3">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>1006</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>18451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3">
+        <v>39</v>
+      </c>
+      <c r="K3" s="3">
+        <v>33</v>
+      </c>
+      <c r="L3" s="3">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3">
+        <v>36</v>
+      </c>
+      <c r="N3" s="3">
+        <v>21</v>
+      </c>
+      <c r="O3" s="3">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>33</v>
+      </c>
+      <c r="R3" s="3">
+        <v>27</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>433</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>7111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3">
+        <v>33</v>
+      </c>
+      <c r="M4" s="3">
+        <v>34</v>
+      </c>
+      <c r="N4" s="3">
+        <v>31</v>
+      </c>
+      <c r="O4" s="3">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>58</v>
+      </c>
+      <c r="R4" s="3">
+        <v>24</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>437</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>6829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3">
+        <v>15</v>
+      </c>
+      <c r="L5" s="3">
+        <v>18</v>
+      </c>
+      <c r="M5" s="3">
+        <v>33</v>
+      </c>
+      <c r="N5" s="3">
+        <v>21</v>
+      </c>
+      <c r="O5" s="3">
+        <v>13</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>256</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>4477</v>
+      </c>
+    </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3">
         <v>26</v>
       </c>
-      <c r="D6" s="3">
-        <v>47</v>
-      </c>
-      <c r="E6" s="3">
-        <v>26</v>
-      </c>
-      <c r="F6" s="3">
-        <v>37</v>
-      </c>
-      <c r="G6" s="3">
-        <v>42</v>
-      </c>
       <c r="H6" s="3">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3">
-        <v>60</v>
-      </c>
-      <c r="J6" s="3">
-        <v>40</v>
-      </c>
-      <c r="K6" s="3">
-        <v>43</v>
-      </c>
-      <c r="L6" s="3">
-        <v>48</v>
-      </c>
-      <c r="M6" s="3">
-        <v>30</v>
-      </c>
-      <c r="N6" s="3">
-        <v>25</v>
-      </c>
-      <c r="O6" s="3">
-        <v>52</v>
-      </c>
-      <c r="P6" s="3">
-        <v>28</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>41</v>
-      </c>
-      <c r="R6" s="3">
-        <v>40</v>
-      </c>
-      <c r="S6" s="3">
-        <v>34</v>
-      </c>
-      <c r="T6" s="3">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="3">
-        <v>38</v>
-      </c>
-      <c r="W6" s="3">
-        <v>40</v>
-      </c>
-      <c r="X6" s="3">
-        <v>30</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>35</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>27</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>27</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>32</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>44</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="AE6" s="2">
-        <v>1006</v>
+        <v>149</v>
       </c>
       <c r="AF6" s="2">
-        <v>18451</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3">
         <v>32</v>
       </c>
-      <c r="D7" s="3">
-        <v>29</v>
-      </c>
-      <c r="E7" s="3">
-        <v>31</v>
-      </c>
-      <c r="F7" s="3">
-        <v>25</v>
-      </c>
       <c r="G7" s="3">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H7" s="3">
-        <v>23</v>
-      </c>
-      <c r="I7" s="3">
-        <v>25</v>
-      </c>
-      <c r="J7" s="3">
-        <v>39</v>
-      </c>
-      <c r="K7" s="3">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3">
-        <v>21</v>
-      </c>
-      <c r="M7" s="3">
-        <v>36</v>
-      </c>
-      <c r="N7" s="3">
-        <v>21</v>
-      </c>
-      <c r="O7" s="3">
-        <v>14</v>
-      </c>
-      <c r="P7" s="3">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>33</v>
-      </c>
-      <c r="R7" s="3">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>3</v>
@@ -1249,66 +1746,66 @@
         <v>3</v>
       </c>
       <c r="AE7" s="2">
-        <v>433</v>
+        <v>155</v>
       </c>
       <c r="AF7" s="2">
-        <v>7111</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C8" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3">
         <v>23</v>
       </c>
-      <c r="F8" s="3">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3">
-        <v>20</v>
-      </c>
-      <c r="I8" s="3">
-        <v>40</v>
-      </c>
-      <c r="J8" s="3">
-        <v>13</v>
-      </c>
-      <c r="K8" s="3">
-        <v>27</v>
-      </c>
-      <c r="L8" s="3">
-        <v>33</v>
-      </c>
-      <c r="M8" s="3">
-        <v>34</v>
-      </c>
-      <c r="N8" s="3">
-        <v>31</v>
-      </c>
-      <c r="O8" s="3">
-        <v>13</v>
-      </c>
-      <c r="P8" s="3">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>58</v>
-      </c>
-      <c r="R8" s="3">
-        <v>24</v>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>3</v>
@@ -1347,57 +1844,57 @@
         <v>3</v>
       </c>
       <c r="AE8" s="2">
-        <v>437</v>
+        <v>104</v>
       </c>
       <c r="AF8" s="2">
-        <v>6829</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3">
         <v>18</v>
       </c>
-      <c r="G9" s="3">
-        <v>21</v>
-      </c>
-      <c r="H9" s="3">
-        <v>18</v>
-      </c>
-      <c r="I9" s="3">
-        <v>16</v>
-      </c>
-      <c r="J9" s="3">
-        <v>24</v>
-      </c>
-      <c r="K9" s="3">
-        <v>15</v>
-      </c>
-      <c r="L9" s="3">
-        <v>18</v>
-      </c>
-      <c r="M9" s="3">
-        <v>33</v>
-      </c>
-      <c r="N9" s="3">
-        <v>21</v>
-      </c>
-      <c r="O9" s="3">
-        <v>13</v>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>3</v>
@@ -1445,36 +1942,36 @@
         <v>3</v>
       </c>
       <c r="AE9" s="2">
-        <v>256</v>
+        <v>95</v>
       </c>
       <c r="AF9" s="2">
-        <v>4477</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3">
-        <v>21</v>
-      </c>
-      <c r="E10" s="3">
-        <v>29</v>
-      </c>
       <c r="F10" s="3">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G10" s="3">
-        <v>26</v>
-      </c>
-      <c r="H10" s="3">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>3</v>
@@ -1543,36 +2040,36 @@
         <v>3</v>
       </c>
       <c r="AE10" s="2">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="AF10" s="2">
-        <v>2230</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3">
-        <v>32</v>
-      </c>
-      <c r="G11" s="3">
-        <v>33</v>
-      </c>
-      <c r="H11" s="3">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>3</v>
@@ -1641,37 +2138,37 @@
         <v>3</v>
       </c>
       <c r="AE11" s="2">
-        <v>155</v>
+        <v>47</v>
       </c>
       <c r="AF11" s="2">
-        <v>2422</v>
+        <v>823</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
         <v>15</v>
       </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3">
-        <v>30</v>
-      </c>
       <c r="E12" s="3">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3">
         <v>21</v>
       </c>
-      <c r="F12" s="3">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="I12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1739,30 +2236,30 @@
         <v>3</v>
       </c>
       <c r="AE12" s="2">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="AF12" s="2">
-        <v>1629</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
       </c>
       <c r="C13" s="3">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F13" s="3">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>3</v>
@@ -1837,33 +2334,33 @@
         <v>3</v>
       </c>
       <c r="AE13" s="2">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="AF13" s="2">
-        <v>1582</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E14" s="3">
-        <v>13</v>
-      </c>
-      <c r="F14" s="3">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>3</v>
@@ -1935,27 +2432,27 @@
         <v>3</v>
       </c>
       <c r="AE14" s="2">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AF14" s="2">
-        <v>1481</v>
+        <v>659</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3">
-        <v>17</v>
-      </c>
-      <c r="E15" s="3">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>3</v>
@@ -2033,58 +2530,58 @@
         <v>3</v>
       </c>
       <c r="AE15" s="2">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="AF15" s="2">
-        <v>823</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3">
         <v>19</v>
-      </c>
-      <c r="B16" s="2">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3">
-        <v>15</v>
-      </c>
-      <c r="E16" s="3">
-        <v>16</v>
       </c>
       <c r="F16" s="3">
         <v>16</v>
       </c>
       <c r="G16" s="3">
+        <v>14</v>
+      </c>
+      <c r="H16" s="3">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3">
+        <v>28</v>
+      </c>
+      <c r="J16" s="3">
+        <v>13</v>
+      </c>
+      <c r="K16" s="3">
+        <v>28</v>
+      </c>
+      <c r="L16" s="3">
+        <v>39</v>
+      </c>
+      <c r="M16" s="3">
+        <v>40</v>
+      </c>
+      <c r="N16" s="3">
+        <v>29</v>
+      </c>
+      <c r="O16" s="3">
         <v>25</v>
       </c>
-      <c r="H16" s="3">
-        <v>21</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="P16" s="3" t="s">
         <v>3</v>
       </c>
@@ -2131,33 +2628,33 @@
         <v>3</v>
       </c>
       <c r="AE16" s="2">
-        <v>113</v>
+        <v>303</v>
       </c>
       <c r="AF16" s="2">
-        <v>1591</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="3">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3">
         <v>26</v>
       </c>
       <c r="E17" s="3">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3">
         <v>17</v>
       </c>
-      <c r="F17" s="3">
-        <v>22</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>3</v>
+      <c r="G17" s="3">
+        <v>20</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>3</v>
@@ -2229,33 +2726,33 @@
         <v>3</v>
       </c>
       <c r="AE17" s="2">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="AF17" s="2">
-        <v>1238</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D18" s="3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E18" s="3">
-        <v>15</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="F18" s="3">
+        <v>19</v>
+      </c>
+      <c r="G18" s="3">
+        <v>14</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>3</v>
@@ -2327,27 +2824,27 @@
         <v>3</v>
       </c>
       <c r="AE18" s="2">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="AF18" s="2">
-        <v>659</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>21</v>
+      </c>
+      <c r="D19" s="3">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>3</v>
+      <c r="E19" s="3">
+        <v>18</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>3</v>
@@ -2425,57 +2922,57 @@
         <v>3</v>
       </c>
       <c r="AE19" s="2">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="AF19" s="2">
-        <v>335</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" s="3">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E20" s="3">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F20" s="3">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G20" s="3">
-        <v>14</v>
-      </c>
-      <c r="H20" s="3">
-        <v>20</v>
-      </c>
-      <c r="I20" s="3">
-        <v>28</v>
-      </c>
-      <c r="J20" s="3">
-        <v>13</v>
-      </c>
-      <c r="K20" s="3">
-        <v>28</v>
-      </c>
-      <c r="L20" s="3">
-        <v>39</v>
-      </c>
-      <c r="M20" s="3">
-        <v>40</v>
-      </c>
-      <c r="N20" s="3">
-        <v>29</v>
-      </c>
-      <c r="O20" s="3">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>3</v>
@@ -2523,33 +3020,33 @@
         <v>3</v>
       </c>
       <c r="AE20" s="2">
-        <v>303</v>
+        <v>105</v>
       </c>
       <c r="AF20" s="2">
-        <v>4953</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21" s="3">
-        <v>27</v>
-      </c>
-      <c r="D21" s="3">
-        <v>26</v>
-      </c>
-      <c r="E21" s="3">
-        <v>18</v>
-      </c>
-      <c r="F21" s="3">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>3</v>
@@ -2621,33 +3118,33 @@
         <v>3</v>
       </c>
       <c r="AE21" s="2">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="AF21" s="2">
-        <v>1742</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C22" s="3">
-        <v>25</v>
-      </c>
-      <c r="D22" s="3">
-        <v>25</v>
-      </c>
-      <c r="E22" s="3">
-        <v>22</v>
-      </c>
-      <c r="F22" s="3">
-        <v>19</v>
-      </c>
-      <c r="G22" s="3">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>3</v>
@@ -2719,27 +3216,27 @@
         <v>3</v>
       </c>
       <c r="AE22" s="2">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="AF22" s="2">
-        <v>1684</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
-        <v>21</v>
-      </c>
-      <c r="D23" s="3">
-        <v>22</v>
-      </c>
-      <c r="E23" s="3">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>3</v>
@@ -2817,85 +3314,85 @@
         <v>3</v>
       </c>
       <c r="AE23" s="2">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="AF23" s="2">
-        <v>1099</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3">
         <v>29</v>
       </c>
       <c r="E24" s="3">
+        <v>22</v>
+      </c>
+      <c r="F24" s="3">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3">
+        <v>14</v>
+      </c>
+      <c r="H24" s="3">
+        <v>17</v>
+      </c>
+      <c r="I24" s="3">
+        <v>17</v>
+      </c>
+      <c r="J24" s="3">
+        <v>13</v>
+      </c>
+      <c r="K24" s="3">
+        <v>21</v>
+      </c>
+      <c r="L24" s="3">
+        <v>11</v>
+      </c>
+      <c r="M24" s="3">
+        <v>19</v>
+      </c>
+      <c r="N24" s="3">
+        <v>17</v>
+      </c>
+      <c r="O24" s="3">
+        <v>18</v>
+      </c>
+      <c r="P24" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>8</v>
+      </c>
+      <c r="R24" s="3">
+        <v>21</v>
+      </c>
+      <c r="S24" s="3">
+        <v>18</v>
+      </c>
+      <c r="T24" s="3">
         <v>24</v>
       </c>
-      <c r="F24" s="3">
+      <c r="U24" s="3">
         <v>21</v>
       </c>
-      <c r="G24" s="3">
+      <c r="V24" s="3">
+        <v>15</v>
+      </c>
+      <c r="W24" s="3">
+        <v>27</v>
+      </c>
+      <c r="X24" s="3">
         <v>21</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X24" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="Y24" s="3" t="s">
         <v>3</v>
       </c>
@@ -2915,500 +3412,10 @@
         <v>3</v>
       </c>
       <c r="AE24" s="2">
-        <v>105</v>
+        <v>404</v>
       </c>
       <c r="AF24" s="2">
-        <v>2141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>13</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE25" s="2">
-        <v>13</v>
-      </c>
-      <c r="AF25" s="2">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>15</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE26" s="2">
-        <v>15</v>
-      </c>
-      <c r="AF26" s="2">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
-        <v>25</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE27" s="2">
-        <v>25</v>
-      </c>
-      <c r="AF27" s="2">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="2">
-        <v>22</v>
-      </c>
-      <c r="C28" s="3">
-        <v>20</v>
-      </c>
-      <c r="D28" s="3">
-        <v>29</v>
-      </c>
-      <c r="E28" s="3">
-        <v>22</v>
-      </c>
-      <c r="F28" s="3">
-        <v>11</v>
-      </c>
-      <c r="G28" s="3">
-        <v>14</v>
-      </c>
-      <c r="H28" s="3">
-        <v>17</v>
-      </c>
-      <c r="I28" s="3">
-        <v>17</v>
-      </c>
-      <c r="J28" s="3">
-        <v>13</v>
-      </c>
-      <c r="K28" s="3">
-        <v>21</v>
-      </c>
-      <c r="L28" s="3">
-        <v>11</v>
-      </c>
-      <c r="M28" s="3">
-        <v>19</v>
-      </c>
-      <c r="N28" s="3">
-        <v>17</v>
-      </c>
-      <c r="O28" s="3">
-        <v>18</v>
-      </c>
-      <c r="P28" s="3">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="3">
-        <v>8</v>
-      </c>
-      <c r="R28" s="3">
-        <v>21</v>
-      </c>
-      <c r="S28" s="3">
-        <v>18</v>
-      </c>
-      <c r="T28" s="3">
-        <v>24</v>
-      </c>
-      <c r="U28" s="3">
-        <v>21</v>
-      </c>
-      <c r="V28" s="3">
-        <v>15</v>
-      </c>
-      <c r="W28" s="3">
-        <v>27</v>
-      </c>
-      <c r="X28" s="3">
-        <v>21</v>
-      </c>
-      <c r="Y28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE28" s="2">
-        <v>404</v>
-      </c>
-      <c r="AF28" s="2">
         <v>9852</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="2">
-        <v>260</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="X29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE29" s="2">
-        <v>7956</v>
-      </c>
-      <c r="AF29" s="4">
-        <v>138020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>